<commit_message>
Re-created all tables and set all keys
</commit_message>
<xml_diff>
--- a/databaseHeading.xlsx
+++ b/databaseHeading.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
   <si>
     <t>vendor_id</t>
   </si>
@@ -63,30 +63,6 @@
     <t>PRODUCT MAIN TABLE</t>
   </si>
   <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>user_name</t>
-  </si>
-  <si>
-    <t>user_email</t>
-  </si>
-  <si>
-    <t>user_password</t>
-  </si>
-  <si>
-    <t>user_contact</t>
-  </si>
-  <si>
-    <t>user_state</t>
-  </si>
-  <si>
-    <t>user_city</t>
-  </si>
-  <si>
-    <t>USER CART TABLE</t>
-  </si>
-  <si>
     <t>USE INNER JOIN</t>
   </si>
   <si>
@@ -96,18 +72,12 @@
     <t>cart_id</t>
   </si>
   <si>
-    <t>cart_user_id</t>
-  </si>
-  <si>
     <t>cart_product_quantity</t>
   </si>
   <si>
     <t>cart_total_price</t>
   </si>
   <si>
-    <t>FK user_id &amp; product_id</t>
-  </si>
-  <si>
     <t>cart_product_id</t>
   </si>
   <si>
@@ -126,27 +96,6 @@
     <t>order_cart_id</t>
   </si>
   <si>
-    <t>order_cust_name</t>
-  </si>
-  <si>
-    <t>order_ship_address</t>
-  </si>
-  <si>
-    <t>order_ship_city</t>
-  </si>
-  <si>
-    <t>order_ship_state</t>
-  </si>
-  <si>
-    <t>order_ship_zip</t>
-  </si>
-  <si>
-    <t>order_cust_contact</t>
-  </si>
-  <si>
-    <t>order_cust_email</t>
-  </si>
-  <si>
     <t>order_tracking_id (AUTO GENERATE)</t>
   </si>
   <si>
@@ -174,30 +123,12 @@
     <t>agent_city</t>
   </si>
   <si>
-    <t>track_id</t>
-  </si>
-  <si>
-    <t>track_tracking_id</t>
-  </si>
-  <si>
-    <t>track_agent_id</t>
-  </si>
-  <si>
-    <t>track_order_id</t>
-  </si>
-  <si>
-    <t>track_order_status</t>
-  </si>
-  <si>
     <t>FK agent_id &amp; order_id</t>
   </si>
   <si>
     <t>VENDOR DETAIL TABLE</t>
   </si>
   <si>
-    <t>USER DETAIL TABLE</t>
-  </si>
-  <si>
     <t>USE REMOVE FUNCTION ALSO</t>
   </si>
   <si>
@@ -210,12 +141,6 @@
     <t>vendor_name</t>
   </si>
   <si>
-    <t>order_delivery_date</t>
-  </si>
-  <si>
-    <t>order_delivery_status</t>
-  </si>
-  <si>
     <t>AGENT DETAIL TABLE</t>
   </si>
   <si>
@@ -250,6 +175,78 @@
   </si>
   <si>
     <t>track_expect_date</t>
+  </si>
+  <si>
+    <t>CUSTOMER DETAIL TABLE</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>customer_name</t>
+  </si>
+  <si>
+    <t>customer_email</t>
+  </si>
+  <si>
+    <t>customer_password</t>
+  </si>
+  <si>
+    <t>customer_contact</t>
+  </si>
+  <si>
+    <t>customer_state</t>
+  </si>
+  <si>
+    <t>customer_city</t>
+  </si>
+  <si>
+    <t>CUSTOMER CART TABLE</t>
+  </si>
+  <si>
+    <t>cart_customer_id</t>
+  </si>
+  <si>
+    <t>FK customer_id &amp; product_id</t>
+  </si>
+  <si>
+    <t>cart_customer_name</t>
+  </si>
+  <si>
+    <t>order_customer_id</t>
+  </si>
+  <si>
+    <t>order_delivery_name</t>
+  </si>
+  <si>
+    <t>order_delivery_contact</t>
+  </si>
+  <si>
+    <t>order_delivery_address</t>
+  </si>
+  <si>
+    <t>order_delivery_city</t>
+  </si>
+  <si>
+    <t>order_delivery_state</t>
+  </si>
+  <si>
+    <t>FK customer_id &amp; cart_id</t>
+  </si>
+  <si>
+    <t>tracking_id</t>
+  </si>
+  <si>
+    <t>tracking_track_id</t>
+  </si>
+  <si>
+    <t>tracking_order_id</t>
+  </si>
+  <si>
+    <t>tracking_agent_id</t>
+  </si>
+  <si>
+    <t>track_delivery_status</t>
   </si>
 </sst>
 </file>
@@ -408,6 +405,15 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -415,15 +421,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -729,15 +726,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.85546875" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="40.140625" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
@@ -752,21 +749,21 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="13"/>
+      <c r="B2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="10"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -782,7 +779,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -796,40 +793,40 @@
     </row>
     <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="13"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="10"/>
     </row>
     <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>12</v>
@@ -837,21 +834,21 @@
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="13"/>
+      <c r="B8" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="10"/>
     </row>
     <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
@@ -870,368 +867,359 @@
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="13"/>
+      <c r="B11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="10"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="13"/>
+      <c r="B14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="10"/>
     </row>
     <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="L15" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="10"/>
+      <c r="B17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="13"/>
     </row>
     <row r="18" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G18" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="10"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="13"/>
+    </row>
+    <row r="21" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="F21" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="G21" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="I21" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="J21" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="K21" t="s">
-        <v>39</v>
-      </c>
-      <c r="L21" t="s">
-        <v>40</v>
-      </c>
-      <c r="M21" t="s">
-        <v>65</v>
-      </c>
-      <c r="N21" t="s">
-        <v>64</v>
+        <v>70</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="10"/>
+      <c r="B23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="13"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" t="s">
         <v>47</v>
       </c>
-      <c r="E24" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" t="s">
-        <v>72</v>
-      </c>
       <c r="G24" s="5" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="H24" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="I24" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="10"/>
+      <c r="B26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="13"/>
     </row>
     <row r="27" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="G27" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="H27" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="10"/>
+      <c r="B29" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="13"/>
     </row>
     <row r="30" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="10"/>
+      <c r="B32" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="13"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="D33" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="E33" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="F33" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B32:N32"/>
+    <mergeCell ref="B29:N29"/>
+    <mergeCell ref="B20:N20"/>
+    <mergeCell ref="B11:N11"/>
+    <mergeCell ref="B8:N8"/>
     <mergeCell ref="B5:N5"/>
     <mergeCell ref="B23:N23"/>
     <mergeCell ref="B26:N26"/>
     <mergeCell ref="B2:N2"/>
     <mergeCell ref="B17:N17"/>
     <mergeCell ref="B14:N14"/>
-    <mergeCell ref="B32:N32"/>
-    <mergeCell ref="B29:N29"/>
-    <mergeCell ref="B20:N20"/>
-    <mergeCell ref="B11:N11"/>
-    <mergeCell ref="B8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
All CRUD complete only admin left
</commit_message>
<xml_diff>
--- a/databaseHeading.xlsx
+++ b/databaseHeading.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
   <si>
     <t>vendor_id</t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>track_delivery_status</t>
+  </si>
+  <si>
+    <t>order_tracking_id</t>
+  </si>
+  <si>
+    <t>ORDER DISPLAY TABLE FOR AGENT(SHORT)</t>
+  </si>
+  <si>
+    <t>ORDER DISPLAY TABLE FOR AGENT (DETAIL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">order_tracking_id </t>
   </si>
 </sst>
 </file>
@@ -405,6 +417,15 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -412,15 +433,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -724,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N33"/>
+  <dimension ref="B1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,21 +761,21 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="10"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="13"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -793,21 +805,21 @@
     </row>
     <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="10"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="13"/>
     </row>
     <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -834,21 +846,21 @@
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="10"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="13"/>
     </row>
     <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
@@ -875,21 +887,21 @@
     </row>
     <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="10"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="13"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -916,21 +928,21 @@
     </row>
     <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="10"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="13"/>
     </row>
     <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
@@ -954,21 +966,21 @@
     </row>
     <row r="16" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="13"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="10"/>
     </row>
     <row r="18" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
@@ -995,21 +1007,21 @@
     </row>
     <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="13"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="10"/>
     </row>
     <row r="21" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
@@ -1048,21 +1060,21 @@
     </row>
     <row r="22" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="13"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="10"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -1092,134 +1104,215 @@
     </row>
     <row r="25" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="13"/>
-    </row>
-    <row r="27" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="10"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>73</v>
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E27" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" t="s">
-        <v>39</v>
-      </c>
-      <c r="H27" t="s">
-        <v>76</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>35</v>
+        <v>69</v>
+      </c>
+      <c r="F27" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="13"/>
-    </row>
-    <row r="30" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="7" t="s">
+      <c r="B29" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="10"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>15</v>
+      <c r="G30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" t="s">
+        <v>69</v>
+      </c>
+      <c r="I30" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="10"/>
+    </row>
+    <row r="33" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G33" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" t="s">
+        <v>76</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="10"/>
+    </row>
+    <row r="36" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="13"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="10"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>43</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C39" t="s">
         <v>44</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D39" t="s">
         <v>48</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E39" t="s">
         <v>45</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F39" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="B23:N23"/>
     <mergeCell ref="B32:N32"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B17:N17"/>
+    <mergeCell ref="B14:N14"/>
+    <mergeCell ref="B26:N26"/>
     <mergeCell ref="B29:N29"/>
+    <mergeCell ref="B38:N38"/>
+    <mergeCell ref="B35:N35"/>
     <mergeCell ref="B20:N20"/>
     <mergeCell ref="B11:N11"/>
     <mergeCell ref="B8:N8"/>
-    <mergeCell ref="B5:N5"/>
-    <mergeCell ref="B23:N23"/>
-    <mergeCell ref="B26:N26"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B17:N17"/>
-    <mergeCell ref="B14:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>